<commit_message>
How to get and update the data from excel based on filter search criteria
</commit_message>
<xml_diff>
--- a/updatedFile.xlsx
+++ b/updatedFile.xlsx
@@ -37,7 +37,7 @@
     <t>Summer</t>
   </si>
   <si>
-    <t>Iphone</t>
+    <t>Apple</t>
   </si>
   <si>
     <t>Red</t>
@@ -475,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>

</xml_diff>